<commit_message>
More builds and item sets update
</commit_message>
<xml_diff>
--- a/bin/data/best-sets_TFT.xlsx
+++ b/bin/data/best-sets_TFT.xlsx
@@ -5111,10 +5111,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F27" sqref="F27"/>
-      <selection pane="bottomLeft" activeCell="AH12" sqref="AH12"/>
+      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7401,11 +7401,11 @@
       </c>
       <c r="F14" s="13" t="str">
         <f>CONCATENATE("""",VLOOKUP($H14,ITEMS!$A$2:$E$57,5,0)," / ",VLOOKUP($I14,ITEMS!$A$2:$E$57,5,0)," / ",VLOOKUP($J14,ITEMS!$A$2:$E$57,5,0),"""")</f>
-        <v>"Life Steal / Critical Damage / Critical Chance / Attack Speed / Buffer (Double Range)"</v>
+        <v>"Life Steal / Critical Damage / Critical Chance / Attack Speed"</v>
       </c>
       <c r="G14" s="13" t="str">
         <f>CONCATENATE("""",VLOOKUP($H14,ITEMS!$A$2:$F$57,6,0)," / ",VLOOKUP($I14,ITEMS!$A$2:$F$57,6,0)," / ",VLOOKUP($J14,ITEMS!$A$2:$F$57,6,0),"""")</f>
-        <v>"Roubo de Vida / Dano Crítico / Chance de Crítico / Velocidade de Ataque / Buffer (Dobra Alcance)"</v>
+        <v>"Roubo de Vida / Dano Crítico / Chance de Crítico / Velocidade de Ataque"</v>
       </c>
       <c r="H14" s="25" t="s">
         <v>15</v>
@@ -7414,7 +7414,7 @@
         <v>10</v>
       </c>
       <c r="J14" s="25" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K14" s="13" t="str">
         <f>CONCATENATE("""",VLOOKUP($M14,ITEMS!$A$2:$E$57,5,0)," / ",VLOOKUP($N14,ITEMS!$A$2:$E$57,5,0)," / ",VLOOKUP($O14,ITEMS!$A$2:$E$57,5,0),"""")</f>
@@ -7460,11 +7460,11 @@
       </c>
       <c r="W14" s="27">
         <f>VLOOKUP(J14,ITEMS!$A$2:$C$57,3,0)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="X14" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>[16,19,22]</v>
+        <v>[16,19,23]</v>
       </c>
       <c r="Y14" s="27">
         <f>VLOOKUP(M14,ITEMS!$A$2:$C$57,3,0)</f>
@@ -7502,8 +7502,8 @@
         <f t="shared" si="3"/>
         <v>"bestSets": [
         {
-          "name": "Life Steal / Critical Damage / Critical Chance / Attack Speed / Buffer (Double Range)",
-          "items": [16,19,22]
+          "name": "Life Steal / Critical Damage / Critical Chance / Attack Speed",
+          "items": [16,19,23]
         },
         {
           "name": "Attack Speed / Attack Speed / Buffer (Double Range) / Life Steal",
@@ -7519,8 +7519,8 @@
         <f t="shared" si="4"/>
         <v>"bestSets": [
         {
-          "name": "Life Steal / Critical Damage / Critical Chance / Attack Speed / Buffer (Double Range)",
-          "items": [16,19,22]
+          "name": "Life Steal / Critical Damage / Critical Chance / Attack Speed",
+          "items": [16,19,23]
         },
         {
           "name": "Attack Speed / Attack Speed / Buffer (Double Range) / Life Steal",
@@ -7536,8 +7536,8 @@
         <f t="shared" si="5"/>
         <v>"bestSets": [
         {
-          "name": "Roubo de Vida / Dano Crítico / Chance de Crítico / Velocidade de Ataque / Buffer (Dobra Alcance)",
-          "items": [16,19,22]
+          "name": "Roubo de Vida / Dano Crítico / Chance de Crítico / Velocidade de Ataque",
+          "items": [16,19,23]
         },
         {
           "name": "Velocidade de Ataque / Velocidade de Ataque / Buffer (Dobra Alcance) / Roubo de Vida",
@@ -7553,8 +7553,8 @@
         <f t="shared" si="6"/>
         <v>"bestSets": [
         {
-          "name": "Roubo de Vida / Dano Crítico / Chance de Crítico / Velocidade de Ataque / Buffer (Dobra Alcance)",
-          "items": [16,19,22]
+          "name": "Roubo de Vida / Dano Crítico / Chance de Crítico / Velocidade de Ataque",
+          "items": [16,19,23]
         },
         {
           "name": "Velocidade de Ataque / Velocidade de Ataque / Buffer (Dobra Alcance) / Roubo de Vida",
@@ -13056,7 +13056,7 @@
       <c r="AK45" s="3"/>
       <c r="AL45" s="5"/>
     </row>
-    <row r="46" spans="1:38" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:38" s="2" customFormat="1" ht="225" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46"/>

</xml_diff>